<commit_message>
All paths changed to if else statement to take into account ypinstaller
</commit_message>
<xml_diff>
--- a/Restored To Eden/Formulation Templates/Night Cream Worksheet.xlsx
+++ b/Restored To Eden/Formulation Templates/Night Cream Worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\Desktop\Haydens commit\ingredient-sorter-master\Restored To Eden\Formulation Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\source\repos\ingredient-sorter\Restored To Eden\Formulation Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34430A7-1D57-4EC5-B1F1-C2C88F8F6690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0067B3F4-93E6-4205-BED2-B82A921DF697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="-13725" windowWidth="27435" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="-15720" windowWidth="17130" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Customer Name</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>COPY DETAILS AND PASTE INTO FORMULATION CALCULATOR</t>
-  </si>
-  <si>
-    <t>Need Analysis</t>
   </si>
 </sst>
 </file>
@@ -653,9 +650,9 @@
   </sheetPr>
   <dimension ref="A1:AB992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -854,9 +851,7 @@
       <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="F6" s="14"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>

</xml_diff>